<commit_message>
Added Chuachard, Klasnja, and Harish working paper
</commit_message>
<xml_diff>
--- a/data/study_results.xlsx
+++ b/data/study_results.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trevorincerti/Box Sync/Projects/corruption_meta/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trevorincerti/gitrepos/corruption_meta/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE2CAB4E-64D7-A149-8F0F-B695D75150A2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79BD499E-8277-E44F-96F7-D917A4A356BB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{F5F3C5B5-0E06-C54A-8CFA-0ED5F6883E31}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="68">
   <si>
     <t>year</t>
   </si>
@@ -220,6 +220,15 @@
   </si>
   <si>
     <t>SEs for unkown. Estimated from chart CIs.</t>
+  </si>
+  <si>
+    <t>Chauchard, Klasnja, and Harris</t>
+  </si>
+  <si>
+    <t>Chauchard et al.</t>
+  </si>
+  <si>
+    <t>Sample size and SEs unknown. Estimated from chart CIs.</t>
   </si>
 </sst>
 </file>
@@ -572,7 +581,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF0ABE20-0DDA-1E4C-A8FF-EDF84ECD427A}">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
@@ -1204,19 +1213,41 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>52</v>
+        <v>11</v>
       </c>
       <c r="B20">
-        <v>2007</v>
+        <v>2017</v>
       </c>
       <c r="C20" t="s">
-        <v>53</v>
+        <v>65</v>
+      </c>
+      <c r="D20" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" t="s">
+        <v>26</v>
       </c>
       <c r="F20">
-        <v>-0.252</v>
+        <v>-0.13</v>
+      </c>
+      <c r="G20">
+        <f>(H20-F20)/-1.96</f>
+        <v>2.0408163265306128E-2</v>
+      </c>
+      <c r="H20">
+        <v>-0.17</v>
+      </c>
+      <c r="I20">
+        <v>-0.09</v>
+      </c>
+      <c r="J20" s="1">
+        <v>1020</v>
       </c>
       <c r="K20" s="1">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="L20" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
@@ -1224,27 +1255,44 @@
         <v>52</v>
       </c>
       <c r="B21">
+        <v>2007</v>
+      </c>
+      <c r="C21" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21">
+        <v>-0.252</v>
+      </c>
+      <c r="K21" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22">
         <v>2018</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>54</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D22" t="s">
         <v>55</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E22" t="s">
         <v>30</v>
       </c>
-      <c r="F21">
+      <c r="F22">
         <v>-0.39200000000000002</v>
       </c>
-      <c r="G21">
+      <c r="G22">
         <v>0.16300000000000001</v>
       </c>
-      <c r="J21">
+      <c r="J22">
         <v>1168</v>
       </c>
-      <c r="K21" s="1">
+      <c r="K22" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated to include full replication of Eggers et al.
</commit_message>
<xml_diff>
--- a/data/study_results.xlsx
+++ b/data/study_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trevorincerti/gitrepos/corruption_meta/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79BD499E-8277-E44F-96F7-D917A4A356BB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4511A244-C169-7F43-84FB-43451C314836}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{F5F3C5B5-0E06-C54A-8CFA-0ED5F6883E31}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="65">
   <si>
     <t>year</t>
   </si>
@@ -111,12 +111,6 @@
     <t>No screener</t>
   </si>
   <si>
-    <t>Eggers, Vivyan, and Wagner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conjoint with multiple choice tasks. N is respondents. </t>
-  </si>
-  <si>
     <t>UK</t>
   </si>
   <si>
@@ -145,9 +139,6 @@
   </si>
   <si>
     <t>De Figueiredo et al. (DEM/PFL)</t>
-  </si>
-  <si>
-    <t>Eggers et al.</t>
   </si>
   <si>
     <t>Mexico</t>
@@ -581,9 +572,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF0ABE20-0DDA-1E4C-A8FF-EDF84ECD427A}">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -604,7 +597,7 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E1" t="s">
         <v>23</v>
@@ -616,16 +609,16 @@
         <v>8</v>
       </c>
       <c r="H1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="I1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="J1" t="s">
         <v>3</v>
       </c>
       <c r="K1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="L1" t="s">
         <v>10</v>
@@ -671,10 +664,10 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F3">
         <v>3.4000000000000002E-2</v>
@@ -700,7 +693,7 @@
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E4" t="s">
         <v>26</v>
@@ -729,10 +722,10 @@
         <v>2010</v>
       </c>
       <c r="C5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E5" t="s">
         <v>26</v>
@@ -750,7 +743,7 @@
         <v>0</v>
       </c>
       <c r="L5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -764,7 +757,7 @@
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E6" t="s">
         <v>24</v>
@@ -793,10 +786,10 @@
         <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F7">
         <v>1.0999999999999999E-2</v>
@@ -825,10 +818,10 @@
         <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F8">
         <v>-3.4000000000000002E-2</v>
@@ -857,10 +850,10 @@
         <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F9">
         <v>-4.3E-3</v>
@@ -886,7 +879,7 @@
         <v>20</v>
       </c>
       <c r="D10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E10" t="s">
         <v>24</v>
@@ -915,7 +908,7 @@
         <v>21</v>
       </c>
       <c r="D11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E11" t="s">
         <v>24</v>
@@ -944,7 +937,7 @@
         <v>12</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E12" t="s">
         <v>24</v>
@@ -962,7 +955,7 @@
         <v>1</v>
       </c>
       <c r="L12" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
@@ -1010,7 +1003,7 @@
         <v>25</v>
       </c>
       <c r="D14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E14" t="s">
         <v>26</v>
@@ -1033,31 +1026,30 @@
         <v>11</v>
       </c>
       <c r="B15">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="C15" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="D15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" t="s">
         <v>40</v>
       </c>
-      <c r="E15" t="s">
-        <v>30</v>
-      </c>
       <c r="F15">
-        <v>-0.24</v>
+        <f>-1.18/6</f>
+        <v>-0.19666666666666666</v>
       </c>
       <c r="G15">
-        <v>1.0999999999999999E-2</v>
+        <f>0.11/6</f>
+        <v>1.8333333333333333E-2</v>
       </c>
       <c r="J15">
-        <v>1367</v>
+        <v>1308</v>
       </c>
       <c r="K15">
-        <v>1</v>
-      </c>
-      <c r="L15" t="s">
-        <v>29</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
@@ -1065,30 +1057,39 @@
         <v>11</v>
       </c>
       <c r="B16">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="C16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D16" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E16" t="s">
         <v>43</v>
       </c>
       <c r="F16">
-        <f>-1.18/6</f>
-        <v>-0.19666666666666666</v>
+        <v>-0.3</v>
       </c>
       <c r="G16">
-        <f>0.11/6</f>
-        <v>1.8333333333333333E-2</v>
-      </c>
-      <c r="J16">
-        <v>1308</v>
-      </c>
-      <c r="K16">
-        <v>0</v>
+        <f>(H16-F16)/-1.96</f>
+        <v>2.5510204081632647E-2</v>
+      </c>
+      <c r="H16">
+        <v>-0.35</v>
+      </c>
+      <c r="I16">
+        <v>-0.25</v>
+      </c>
+      <c r="J16" s="1">
+        <f>8668/3</f>
+        <v>2889.3333333333335</v>
+      </c>
+      <c r="K16" s="1">
+        <v>1</v>
+      </c>
+      <c r="L16" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
@@ -1099,26 +1100,26 @@
         <v>2017</v>
       </c>
       <c r="C17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" t="s">
         <v>45</v>
       </c>
-      <c r="D17" t="s">
-        <v>49</v>
-      </c>
-      <c r="E17" t="s">
-        <v>46</v>
-      </c>
       <c r="F17">
-        <v>-0.3</v>
+        <v>-0.42</v>
       </c>
       <c r="G17">
         <f>(H17-F17)/-1.96</f>
         <v>2.5510204081632647E-2</v>
       </c>
       <c r="H17">
-        <v>-0.35</v>
+        <v>-0.47</v>
       </c>
       <c r="I17">
-        <v>-0.25</v>
+        <v>-0.37</v>
       </c>
       <c r="J17" s="1">
         <f>8668/3</f>
@@ -1128,7 +1129,7 @@
         <v>1</v>
       </c>
       <c r="L17" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
@@ -1139,26 +1140,26 @@
         <v>2017</v>
       </c>
       <c r="C18" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D18" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E18" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F18">
-        <v>-0.42</v>
+        <v>-0.34</v>
       </c>
       <c r="G18">
         <f>(H18-F18)/-1.96</f>
         <v>2.5510204081632647E-2</v>
       </c>
       <c r="H18">
-        <v>-0.47</v>
+        <v>-0.39</v>
       </c>
       <c r="I18">
-        <v>-0.37</v>
+        <v>-0.28999999999999998</v>
       </c>
       <c r="J18" s="1">
         <f>8668/3</f>
@@ -1168,7 +1169,7 @@
         <v>1</v>
       </c>
       <c r="L18" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
@@ -1179,120 +1180,80 @@
         <v>2017</v>
       </c>
       <c r="C19" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="D19" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="E19" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="F19">
-        <v>-0.34</v>
+        <v>-0.13</v>
       </c>
       <c r="G19">
         <f>(H19-F19)/-1.96</f>
-        <v>2.5510204081632647E-2</v>
+        <v>2.0408163265306128E-2</v>
       </c>
       <c r="H19">
-        <v>-0.39</v>
+        <v>-0.17</v>
       </c>
       <c r="I19">
-        <v>-0.28999999999999998</v>
+        <v>-0.09</v>
       </c>
       <c r="J19" s="1">
-        <f>8668/3</f>
-        <v>2889.3333333333335</v>
+        <v>1020</v>
       </c>
       <c r="K19" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L19" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="B20">
-        <v>2017</v>
+        <v>2007</v>
       </c>
       <c r="C20" t="s">
-        <v>65</v>
-      </c>
-      <c r="D20" t="s">
-        <v>66</v>
-      </c>
-      <c r="E20" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="F20">
-        <v>-0.13</v>
-      </c>
-      <c r="G20">
-        <f>(H20-F20)/-1.96</f>
-        <v>2.0408163265306128E-2</v>
-      </c>
-      <c r="H20">
-        <v>-0.17</v>
-      </c>
-      <c r="I20">
-        <v>-0.09</v>
-      </c>
-      <c r="J20" s="1">
-        <v>1020</v>
+        <v>-0.252</v>
       </c>
       <c r="K20" s="1">
-        <v>0</v>
-      </c>
-      <c r="L20" t="s">
-        <v>67</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21">
+        <v>2018</v>
+      </c>
+      <c r="C21" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" t="s">
         <v>52</v>
       </c>
-      <c r="B21">
-        <v>2007</v>
-      </c>
-      <c r="C21" t="s">
-        <v>53</v>
+      <c r="E21" t="s">
+        <v>28</v>
       </c>
       <c r="F21">
-        <v>-0.252</v>
+        <v>-0.39200000000000002</v>
+      </c>
+      <c r="G21">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="J21">
+        <v>1168</v>
       </c>
       <c r="K21" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>52</v>
-      </c>
-      <c r="B22">
-        <v>2018</v>
-      </c>
-      <c r="C22" t="s">
-        <v>54</v>
-      </c>
-      <c r="D22" t="s">
-        <v>55</v>
-      </c>
-      <c r="E22" t="s">
-        <v>30</v>
-      </c>
-      <c r="F22">
-        <v>-0.39200000000000002</v>
-      </c>
-      <c r="G22">
-        <v>0.16300000000000001</v>
-      </c>
-      <c r="J22">
-        <v>1168</v>
-      </c>
-      <c r="K22" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added lab experiment point estimates to appendix
</commit_message>
<xml_diff>
--- a/data/study_results.xlsx
+++ b/data/study_results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10412"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trevorincerti/gitrepos/corruption_meta/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4511A244-C169-7F43-84FB-43451C314836}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E8C1852-7246-9543-B663-AD0BC0125833}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{F5F3C5B5-0E06-C54A-8CFA-0ED5F6883E31}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="66">
   <si>
     <t>year</t>
   </si>
@@ -177,9 +177,6 @@
     <t>Lab</t>
   </si>
   <si>
-    <t>Azfar &amp; Nelson</t>
-  </si>
-  <si>
     <t>Solaz, De Vries, &amp; de Geus</t>
   </si>
   <si>
@@ -220,6 +217,12 @@
   </si>
   <si>
     <t>Sample size and SEs unknown. Estimated from chart CIs.</t>
+  </si>
+  <si>
+    <t>Arvate &amp; Mittlaender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N is number of respondents. Ten rounds. SE clustered by respondent. </t>
   </si>
 </sst>
 </file>
@@ -574,9 +577,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF0ABE20-0DDA-1E4C-A8FF-EDF84ECD427A}">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -609,16 +610,16 @@
         <v>8</v>
       </c>
       <c r="H1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I1" t="s">
         <v>58</v>
-      </c>
-      <c r="I1" t="s">
-        <v>59</v>
       </c>
       <c r="J1" t="s">
         <v>3</v>
       </c>
       <c r="K1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L1" t="s">
         <v>10</v>
@@ -693,7 +694,7 @@
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E4" t="s">
         <v>26</v>
@@ -722,10 +723,10 @@
         <v>2010</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E5" t="s">
         <v>26</v>
@@ -743,7 +744,7 @@
         <v>0</v>
       </c>
       <c r="L5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -955,7 +956,7 @@
         <v>1</v>
       </c>
       <c r="L12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
@@ -1089,7 +1090,7 @@
         <v>1</v>
       </c>
       <c r="L16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
@@ -1129,7 +1130,7 @@
         <v>1</v>
       </c>
       <c r="L17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
@@ -1169,7 +1170,7 @@
         <v>1</v>
       </c>
       <c r="L18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
@@ -1180,10 +1181,10 @@
         <v>2017</v>
       </c>
       <c r="C19" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" t="s">
         <v>62</v>
-      </c>
-      <c r="D19" t="s">
-        <v>63</v>
       </c>
       <c r="E19" t="s">
         <v>26</v>
@@ -1208,7 +1209,7 @@
         <v>0</v>
       </c>
       <c r="L19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
@@ -1216,13 +1217,25 @@
         <v>49</v>
       </c>
       <c r="B20">
-        <v>2007</v>
+        <v>2018</v>
       </c>
       <c r="C20" t="s">
         <v>50</v>
       </c>
+      <c r="D20" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" t="s">
+        <v>28</v>
+      </c>
       <c r="F20">
-        <v>-0.252</v>
+        <v>-0.39200000000000002</v>
+      </c>
+      <c r="G20">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="J20">
+        <v>1168</v>
       </c>
       <c r="K20" s="1">
         <v>1</v>
@@ -1233,28 +1246,31 @@
         <v>49</v>
       </c>
       <c r="B21">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="C21" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="D21" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="E21" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F21">
-        <v>-0.39200000000000002</v>
+        <v>-0.46</v>
       </c>
       <c r="G21">
-        <v>0.16300000000000001</v>
+        <v>0.16</v>
       </c>
       <c r="J21">
-        <v>1168</v>
+        <v>80</v>
       </c>
       <c r="K21" s="1">
         <v>1</v>
+      </c>
+      <c r="L21" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Wordsmithing and added reported p-values to dataset
</commit_message>
<xml_diff>
--- a/data/study_results.xlsx
+++ b/data/study_results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10412"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trevorincerti/gitrepos/corruption_meta/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D0B5E97-0756-6240-A9C2-0674795A6335}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{050E21F4-BE61-2B4E-ADE4-83F7599FD5DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{F5F3C5B5-0E06-C54A-8CFA-0ED5F6883E31}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="71">
   <si>
     <t>year</t>
   </si>
@@ -223,6 +223,21 @@
   </si>
   <si>
     <t xml:space="preserve">N is number of respondents. Ten rounds. SE clustered by respondent. </t>
+  </si>
+  <si>
+    <t>p_reported</t>
+  </si>
+  <si>
+    <t>&gt;0.1</t>
+  </si>
+  <si>
+    <t>&lt;0.1</t>
+  </si>
+  <si>
+    <t>&lt;0.01</t>
+  </si>
+  <si>
+    <t>&lt;0.05</t>
   </si>
 </sst>
 </file>
@@ -575,7 +590,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF0ABE20-0DDA-1E4C-A8FF-EDF84ECD427A}">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
@@ -584,10 +599,10 @@
     <col min="3" max="3" width="45.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="57.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="57.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -616,16 +631,19 @@
         <v>58</v>
       </c>
       <c r="J1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K1" t="s">
         <v>3</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>56</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -647,14 +665,17 @@
       <c r="G2">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="J2">
+      <c r="J2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K2">
         <v>264</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -676,14 +697,17 @@
       <c r="G3">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="J3">
+      <c r="J3" t="s">
+        <v>69</v>
+      </c>
+      <c r="K3">
         <v>268</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -705,17 +729,20 @@
       <c r="G4">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="J4">
+      <c r="J4" t="s">
+        <v>67</v>
+      </c>
+      <c r="K4">
         <v>775</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>0</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -737,17 +764,20 @@
       <c r="G5">
         <v>0.08</v>
       </c>
-      <c r="J5">
+      <c r="J5" t="s">
+        <v>67</v>
+      </c>
+      <c r="K5">
         <v>2028</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>0</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -769,14 +799,17 @@
       <c r="G6">
         <v>0.03</v>
       </c>
-      <c r="J6">
+      <c r="J6" t="s">
+        <v>67</v>
+      </c>
+      <c r="K6">
         <v>818</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -798,17 +831,20 @@
       <c r="G7">
         <v>1.6E-2</v>
       </c>
-      <c r="J7">
+      <c r="J7" t="s">
+        <v>67</v>
+      </c>
+      <c r="K7">
         <v>3131</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>1</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -830,17 +866,20 @@
       <c r="G8">
         <v>1.6E-2</v>
       </c>
-      <c r="J8">
+      <c r="J8" t="s">
+        <v>70</v>
+      </c>
+      <c r="K8">
         <v>2883</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>1</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -862,14 +901,17 @@
       <c r="G9">
         <v>2E-3</v>
       </c>
-      <c r="J9">
+      <c r="J9" t="s">
+        <v>70</v>
+      </c>
+      <c r="K9">
         <v>2340</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -891,14 +933,17 @@
       <c r="G10">
         <v>1.01E-2</v>
       </c>
-      <c r="J10">
+      <c r="J10" t="s">
+        <v>70</v>
+      </c>
+      <c r="K10">
         <v>200</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -920,14 +965,17 @@
       <c r="G11">
         <v>9.4999999999999998E-3</v>
       </c>
-      <c r="J11">
+      <c r="J11" t="s">
+        <v>67</v>
+      </c>
+      <c r="K11">
         <v>200</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -949,17 +997,20 @@
       <c r="G12">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="J12">
+      <c r="J12" t="s">
+        <v>67</v>
+      </c>
+      <c r="K12">
         <v>619</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>1</v>
       </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -983,17 +1034,20 @@
         <f>0.2/6</f>
         <v>3.3333333333333333E-2</v>
       </c>
-      <c r="J13">
+      <c r="J13" t="s">
+        <v>70</v>
+      </c>
+      <c r="K13">
         <v>744</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>0</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -1015,14 +1069,17 @@
       <c r="G14">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="J14">
+      <c r="J14" t="s">
+        <v>69</v>
+      </c>
+      <c r="K14">
         <v>4467</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -1046,14 +1103,17 @@
         <f>0.11/6</f>
         <v>1.8333333333333333E-2</v>
       </c>
-      <c r="J15">
+      <c r="J15" t="s">
+        <v>69</v>
+      </c>
+      <c r="K15">
         <v>1308</v>
       </c>
-      <c r="K15">
+      <c r="L15">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -1082,18 +1142,21 @@
       <c r="I16">
         <v>-0.25</v>
       </c>
-      <c r="J16" s="1">
+      <c r="J16" t="s">
+        <v>69</v>
+      </c>
+      <c r="K16" s="1">
         <f>8668/3</f>
         <v>2889.3333333333335</v>
       </c>
-      <c r="K16" s="1">
+      <c r="L16" s="1">
         <v>1</v>
       </c>
-      <c r="L16" t="s">
+      <c r="M16" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -1122,18 +1185,21 @@
       <c r="I17">
         <v>-0.37</v>
       </c>
-      <c r="J17" s="1">
+      <c r="J17" t="s">
+        <v>69</v>
+      </c>
+      <c r="K17" s="1">
         <f>8668/3</f>
         <v>2889.3333333333335</v>
       </c>
-      <c r="K17" s="1">
+      <c r="L17" s="1">
         <v>1</v>
       </c>
-      <c r="L17" t="s">
+      <c r="M17" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -1162,18 +1228,21 @@
       <c r="I18">
         <v>-0.28999999999999998</v>
       </c>
-      <c r="J18" s="1">
+      <c r="J18" t="s">
+        <v>69</v>
+      </c>
+      <c r="K18" s="1">
         <f>8668/3</f>
         <v>2889.3333333333335</v>
       </c>
-      <c r="K18" s="1">
+      <c r="L18" s="1">
         <v>1</v>
       </c>
-      <c r="L18" t="s">
+      <c r="M18" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -1202,17 +1271,20 @@
       <c r="I19">
         <v>-0.09</v>
       </c>
-      <c r="J19" s="1">
+      <c r="J19" t="s">
+        <v>69</v>
+      </c>
+      <c r="K19" s="1">
         <v>1020</v>
       </c>
-      <c r="K19" s="1">
+      <c r="L19" s="1">
         <v>0</v>
       </c>
-      <c r="L19" t="s">
+      <c r="M19" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>49</v>
       </c>
@@ -1234,14 +1306,17 @@
       <c r="G20">
         <v>0.16300000000000001</v>
       </c>
-      <c r="J20">
+      <c r="J20" t="s">
+        <v>70</v>
+      </c>
+      <c r="K20">
         <v>1168</v>
       </c>
-      <c r="K20" s="1">
+      <c r="L20" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>49</v>
       </c>
@@ -1263,13 +1338,16 @@
       <c r="G21">
         <v>0.16</v>
       </c>
-      <c r="J21">
+      <c r="J21" t="s">
+        <v>69</v>
+      </c>
+      <c r="K21">
         <v>80</v>
       </c>
-      <c r="K21" s="1">
+      <c r="L21" s="1">
         <v>1</v>
       </c>
-      <c r="L21" t="s">
+      <c r="M21" t="s">
         <v>65</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added KLT replication data and re-analyzed data
</commit_message>
<xml_diff>
--- a/data/study_results.xlsx
+++ b/data/study_results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trevorincerti/gitrepos/corruption_meta/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E20582-EA81-A343-A0BC-83945E2E3E82}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77BB5776-0FFD-9C46-9BD0-6D53D5B2FD6A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{F5F3C5B5-0E06-C54A-8CFA-0ED5F6883E31}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="59">
   <si>
     <t>year</t>
   </si>
@@ -141,27 +141,6 @@
     <t>Uganda</t>
   </si>
   <si>
-    <t>Klasna, Lupu, and Tucker</t>
-  </si>
-  <si>
-    <t>Chile</t>
-  </si>
-  <si>
-    <t>Argentina</t>
-  </si>
-  <si>
-    <t>Uruguay</t>
-  </si>
-  <si>
-    <t>Klasna et al. (Chile)</t>
-  </si>
-  <si>
-    <t>Klasna et al. (Uruguay)</t>
-  </si>
-  <si>
-    <t>Klasna et al. (Argentina)</t>
-  </si>
-  <si>
     <t>Lab</t>
   </si>
   <si>
@@ -190,9 +169,6 @@
   </si>
   <si>
     <t>ci_upper</t>
-  </si>
-  <si>
-    <t>Sample size and SEs for country unkown. Estimated from chart CIs.</t>
   </si>
   <si>
     <t>SEs for unkown. Estimated from chart CIs.</t>
@@ -578,11 +554,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF0ABE20-0DDA-1E4C-A8FF-EDF84ECD427A}">
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -615,19 +589,19 @@
         <v>8</v>
       </c>
       <c r="H1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="I1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" t="s">
         <v>54</v>
-      </c>
-      <c r="J1" t="s">
-        <v>62</v>
       </c>
       <c r="K1" t="s">
         <v>3</v>
       </c>
       <c r="L1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="M1" t="s">
         <v>10</v>
@@ -656,7 +630,7 @@
         <v>4.1000000000000002E-2</v>
       </c>
       <c r="J2" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="K2">
         <v>264</v>
@@ -688,7 +662,7 @@
         <v>7.0000000000000001E-3</v>
       </c>
       <c r="J3" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="K3">
         <v>268</v>
@@ -708,7 +682,7 @@
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="E4" t="s">
         <v>25</v>
@@ -720,7 +694,7 @@
         <v>1.0999999999999999E-2</v>
       </c>
       <c r="J4" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="K4">
         <v>775</v>
@@ -740,10 +714,10 @@
         <v>2010</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="D5" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E5" t="s">
         <v>25</v>
@@ -755,7 +729,7 @@
         <v>0.08</v>
       </c>
       <c r="J5" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="K5">
         <v>2028</v>
@@ -764,7 +738,7 @@
         <v>0</v>
       </c>
       <c r="M5" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -790,7 +764,7 @@
         <v>0.03</v>
       </c>
       <c r="J6" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="K6">
         <v>818</v>
@@ -822,7 +796,7 @@
         <v>1.6E-2</v>
       </c>
       <c r="J7" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="K7">
         <v>3131</v>
@@ -857,7 +831,7 @@
         <v>1.6E-2</v>
       </c>
       <c r="J8" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="K8">
         <v>2883</v>
@@ -892,7 +866,7 @@
         <v>2E-3</v>
       </c>
       <c r="J9" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="K9">
         <v>2340</v>
@@ -924,7 +898,7 @@
         <v>1.01E-2</v>
       </c>
       <c r="J10" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="K10">
         <v>200</v>
@@ -956,7 +930,7 @@
         <v>9.4999999999999998E-3</v>
       </c>
       <c r="J11" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="K11">
         <v>200</v>
@@ -988,7 +962,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="J12" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="K12">
         <v>619</v>
@@ -997,7 +971,7 @@
         <v>1</v>
       </c>
       <c r="M12" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
@@ -1023,7 +997,7 @@
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="J13" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="K13">
         <v>4467</v>
@@ -1040,234 +1014,105 @@
         <v>2017</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="D14" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="E14" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="F14">
-        <v>-0.3</v>
+        <v>-0.13</v>
       </c>
       <c r="G14">
         <f>(H14-F14)/-1.96</f>
-        <v>2.5510204081632647E-2</v>
+        <v>2.0408163265306128E-2</v>
       </c>
       <c r="H14">
-        <v>-0.35</v>
+        <v>-0.17</v>
       </c>
       <c r="I14">
-        <v>-0.25</v>
+        <v>-0.09</v>
       </c>
       <c r="J14" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="K14" s="1">
-        <f>8668/3</f>
-        <v>2889.3333333333335</v>
+        <v>1020</v>
       </c>
       <c r="L14" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M14" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="B15">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D15" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E15" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="F15">
-        <v>-0.42</v>
+        <v>-0.39200000000000002</v>
       </c>
       <c r="G15">
-        <f>(H15-F15)/-1.96</f>
-        <v>2.5510204081632647E-2</v>
-      </c>
-      <c r="H15">
-        <v>-0.47</v>
-      </c>
-      <c r="I15">
-        <v>-0.37</v>
+        <v>0.16300000000000001</v>
       </c>
       <c r="J15" t="s">
-        <v>65</v>
-      </c>
-      <c r="K15" s="1">
-        <f>8668/3</f>
-        <v>2889.3333333333335</v>
+        <v>58</v>
+      </c>
+      <c r="K15">
+        <v>1168</v>
       </c>
       <c r="L15" s="1">
         <v>1</v>
       </c>
-      <c r="M15" t="s">
-        <v>55</v>
-      </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="B16">
         <v>2017</v>
       </c>
       <c r="C16" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="D16" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="E16" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="F16">
-        <v>-0.34</v>
+        <v>-0.46</v>
       </c>
       <c r="G16">
-        <f>(H16-F16)/-1.96</f>
-        <v>2.5510204081632647E-2</v>
-      </c>
-      <c r="H16">
-        <v>-0.39</v>
-      </c>
-      <c r="I16">
-        <v>-0.28999999999999998</v>
+        <v>0.16</v>
       </c>
       <c r="J16" t="s">
-        <v>65</v>
-      </c>
-      <c r="K16" s="1">
-        <f>8668/3</f>
-        <v>2889.3333333333335</v>
+        <v>57</v>
+      </c>
+      <c r="K16">
+        <v>80</v>
       </c>
       <c r="L16" s="1">
         <v>1</v>
       </c>
       <c r="M16" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17">
-        <v>2017</v>
-      </c>
-      <c r="C17" t="s">
-        <v>57</v>
-      </c>
-      <c r="D17" t="s">
-        <v>58</v>
-      </c>
-      <c r="E17" t="s">
-        <v>25</v>
-      </c>
-      <c r="F17">
-        <v>-0.13</v>
-      </c>
-      <c r="G17">
-        <f>(H17-F17)/-1.96</f>
-        <v>2.0408163265306128E-2</v>
-      </c>
-      <c r="H17">
-        <v>-0.17</v>
-      </c>
-      <c r="I17">
-        <v>-0.09</v>
-      </c>
-      <c r="J17" t="s">
-        <v>65</v>
-      </c>
-      <c r="K17" s="1">
-        <v>1020</v>
-      </c>
-      <c r="L17" s="1">
-        <v>0</v>
-      </c>
-      <c r="M17" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18">
-        <v>2018</v>
-      </c>
-      <c r="C18" t="s">
-        <v>46</v>
-      </c>
-      <c r="D18" t="s">
-        <v>47</v>
-      </c>
-      <c r="E18" t="s">
-        <v>26</v>
-      </c>
-      <c r="F18">
-        <v>-0.39200000000000002</v>
-      </c>
-      <c r="G18">
-        <v>0.16300000000000001</v>
-      </c>
-      <c r="J18" t="s">
-        <v>66</v>
-      </c>
-      <c r="K18">
-        <v>1168</v>
-      </c>
-      <c r="L18" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>45</v>
-      </c>
-      <c r="B19">
-        <v>2017</v>
-      </c>
-      <c r="C19" t="s">
-        <v>60</v>
-      </c>
-      <c r="D19" t="s">
-        <v>60</v>
-      </c>
-      <c r="E19" t="s">
-        <v>23</v>
-      </c>
-      <c r="F19">
-        <v>-0.46</v>
-      </c>
-      <c r="G19">
-        <v>0.16</v>
-      </c>
-      <c r="J19" t="s">
-        <v>65</v>
-      </c>
-      <c r="K19">
-        <v>80</v>
-      </c>
-      <c r="L19" s="1">
-        <v>1</v>
-      </c>
-      <c r="M19" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Chauchard et al. replication data and removed references to digitally measured plots
</commit_message>
<xml_diff>
--- a/data/study_results.xlsx
+++ b/data/study_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trevorincerti/gitrepos/corruption_meta/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AA27227-A419-2047-BCE7-294E683F8379}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EB79EB9-CC02-8E4C-B4AA-674B78DB0915}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{F5F3C5B5-0E06-C54A-8CFA-0ED5F6883E31}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="55">
   <si>
     <t>year</t>
   </si>
@@ -169,15 +169,6 @@
   </si>
   <si>
     <t>ci_upper</t>
-  </si>
-  <si>
-    <t>Chauchard, Klasnja, and Harris</t>
-  </si>
-  <si>
-    <t>Chauchard et al.</t>
-  </si>
-  <si>
-    <t>Sample size and SEs unknown. Estimated from chart CIs.</t>
   </si>
   <si>
     <t>Arvate &amp; Mittlaender</t>
@@ -551,7 +542,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF0ABE20-0DDA-1E4C-A8FF-EDF84ECD427A}">
-  <dimension ref="A1:M15"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
@@ -592,7 +583,7 @@
         <v>47</v>
       </c>
       <c r="J1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="K1" t="s">
         <v>3</v>
@@ -627,7 +618,7 @@
         <v>4.1000000000000002E-2</v>
       </c>
       <c r="J2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="K2">
         <v>264</v>
@@ -659,7 +650,7 @@
         <v>7.0000000000000001E-3</v>
       </c>
       <c r="J3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="K3">
         <v>268</v>
@@ -691,7 +682,7 @@
         <v>1.0999999999999999E-2</v>
       </c>
       <c r="J4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="K4">
         <v>775</v>
@@ -726,7 +717,7 @@
         <v>0.08</v>
       </c>
       <c r="J5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="K5">
         <v>2028</v>
@@ -761,7 +752,7 @@
         <v>0.03</v>
       </c>
       <c r="J6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="K6">
         <v>818</v>
@@ -793,7 +784,7 @@
         <v>1.6E-2</v>
       </c>
       <c r="J7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="K7">
         <v>3131</v>
@@ -828,7 +819,7 @@
         <v>1.6E-2</v>
       </c>
       <c r="J8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="K8">
         <v>2883</v>
@@ -863,7 +854,7 @@
         <v>2E-3</v>
       </c>
       <c r="J9" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="K9">
         <v>2340</v>
@@ -895,7 +886,7 @@
         <v>1.01E-2</v>
       </c>
       <c r="J10" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="K10">
         <v>200</v>
@@ -927,7 +918,7 @@
         <v>9.4999999999999998E-3</v>
       </c>
       <c r="J11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="K11">
         <v>200</v>
@@ -959,7 +950,7 @@
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="J12" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="K12">
         <v>4467</v>
@@ -970,44 +961,34 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="B13">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="C13" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D13" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="E13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F13">
-        <v>-0.13</v>
+        <v>-0.39200000000000002</v>
       </c>
       <c r="G13">
-        <f>(H13-F13)/-1.96</f>
-        <v>2.0408163265306128E-2</v>
-      </c>
-      <c r="H13">
-        <v>-0.17</v>
-      </c>
-      <c r="I13">
-        <v>-0.09</v>
+        <v>0.16300000000000001</v>
       </c>
       <c r="J13" t="s">
-        <v>56</v>
-      </c>
-      <c r="K13" s="1">
-        <v>1020</v>
+        <v>54</v>
+      </c>
+      <c r="K13">
+        <v>1168</v>
       </c>
       <c r="L13" s="1">
-        <v>0</v>
-      </c>
-      <c r="M13" t="s">
-        <v>50</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
@@ -1015,66 +996,34 @@
         <v>38</v>
       </c>
       <c r="B14">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="D14" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="E14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F14">
-        <v>-0.39200000000000002</v>
+        <v>-0.46</v>
       </c>
       <c r="G14">
-        <v>0.16300000000000001</v>
+        <v>0.16</v>
       </c>
       <c r="J14" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="K14">
-        <v>1168</v>
+        <v>80</v>
       </c>
       <c r="L14" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>38</v>
-      </c>
-      <c r="B15">
-        <v>2017</v>
-      </c>
-      <c r="C15" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" t="s">
-        <v>51</v>
-      </c>
-      <c r="E15" t="s">
-        <v>23</v>
-      </c>
-      <c r="F15">
-        <v>-0.46</v>
-      </c>
-      <c r="G15">
-        <v>0.16</v>
-      </c>
-      <c r="J15" t="s">
-        <v>56</v>
-      </c>
-      <c r="K15">
-        <v>80</v>
-      </c>
-      <c r="L15" s="1">
-        <v>1</v>
-      </c>
-      <c r="M15" t="s">
-        <v>52</v>
+      <c r="M14" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to prose and formatting
</commit_message>
<xml_diff>
--- a/data/study_results.xlsx
+++ b/data/study_results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trevorincerti/gitrepos/corruption_meta/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EB79EB9-CC02-8E4C-B4AA-674B78DB0915}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F554BD0-23C5-E943-8173-E1F52D08C212}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{F5F3C5B5-0E06-C54A-8CFA-0ED5F6883E31}"/>
   </bookViews>
@@ -676,10 +676,10 @@
         <v>25</v>
       </c>
       <c r="F4">
-        <v>4.0000000000000001E-3</v>
+        <v>-1.4999999999999999E-2</v>
       </c>
       <c r="G4">
-        <v>1.0999999999999999E-2</v>
+        <v>2.3E-2</v>
       </c>
       <c r="J4" t="s">
         <v>51</v>

</xml_diff>

<commit_message>
Added all reported p-values to data
</commit_message>
<xml_diff>
--- a/data/study_results.xlsx
+++ b/data/study_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trevorincerti/gitrepos/corruption_meta/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F554BD0-23C5-E943-8173-E1F52D08C212}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED13CF66-C4B5-3C44-8C14-D18C28228B1D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{F5F3C5B5-0E06-C54A-8CFA-0ED5F6883E31}"/>
+    <workbookView xWindow="28800" yWindow="-10320" windowWidth="25600" windowHeight="20020" xr2:uid="{F5F3C5B5-0E06-C54A-8CFA-0ED5F6883E31}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="57">
   <si>
     <t>year</t>
   </si>
@@ -190,6 +190,12 @@
   </si>
   <si>
     <t>&lt;0.05</t>
+  </si>
+  <si>
+    <t>&lt;0.02</t>
+  </si>
+  <si>
+    <t>p_replicated</t>
   </si>
 </sst>
 </file>
@@ -542,7 +548,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF0ABE20-0DDA-1E4C-A8FF-EDF84ECD427A}">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
@@ -551,10 +557,11 @@
     <col min="3" max="3" width="45.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="57.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="57.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -586,16 +593,19 @@
         <v>50</v>
       </c>
       <c r="K1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L1" t="s">
         <v>3</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>45</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -620,14 +630,14 @@
       <c r="J2" t="s">
         <v>52</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>264</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -652,14 +662,14 @@
       <c r="J3" t="s">
         <v>53</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>268</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -684,17 +694,17 @@
       <c r="J4" t="s">
         <v>51</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>775</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>0</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -719,17 +729,17 @@
       <c r="J5" t="s">
         <v>51</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>2028</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>0</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -754,14 +764,14 @@
       <c r="J6" t="s">
         <v>51</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>818</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -786,17 +796,17 @@
       <c r="J7" t="s">
         <v>51</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>3131</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>1</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -819,19 +829,19 @@
         <v>1.6E-2</v>
       </c>
       <c r="J8" t="s">
-        <v>54</v>
-      </c>
-      <c r="K8">
+        <v>55</v>
+      </c>
+      <c r="L8">
         <v>2883</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>1</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -856,14 +866,14 @@
       <c r="J9" t="s">
         <v>54</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>2340</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -888,14 +898,14 @@
       <c r="J10" t="s">
         <v>54</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>200</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -920,14 +930,14 @@
       <c r="J11" t="s">
         <v>51</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>200</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -952,14 +962,14 @@
       <c r="J12" t="s">
         <v>53</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>4467</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -984,14 +994,14 @@
       <c r="J13" t="s">
         <v>54</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>1168</v>
       </c>
-      <c r="L13" s="1">
+      <c r="M13" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -1016,13 +1026,13 @@
       <c r="J14" t="s">
         <v>53</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>80</v>
       </c>
-      <c r="L14" s="1">
+      <c r="M14" s="1">
         <v>1</v>
       </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>